<commit_message>
20170825 - Key events working.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -2184,10 +2184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,107 +2197,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
+      <c r="A1">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2311,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2320,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2340,22 +2259,22 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -2372,22 +2291,22 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2404,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2416,10 +2335,10 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2433,10 +2352,10 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2451,10 +2370,10 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2465,28 +2384,28 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2500,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -2515,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2525,11 +2444,35 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2537,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2558,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2569,25 +2512,25 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -2597,35 +2540,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2633,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2654,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -2764,25 +2683,25 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -2796,25 +2715,25 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -2825,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2846,18 +2765,42 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23">
         <v>0</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2865,25 +2808,25 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2903,19 +2846,19 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2925,35 +2868,11 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
       <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2961,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2993,25 +2912,25 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -3025,10 +2944,10 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -3046,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -3089,10 +3008,10 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -3110,7 +3029,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -3121,25 +3040,25 @@
         <v>0</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -3153,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -3181,11 +3100,35 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34">
         <v>0</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3199,19 +3142,19 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -3225,25 +3168,25 @@
         <v>0</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -3253,35 +3196,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" t="s">
         <v>0</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3289,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -3310,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -3420,25 +3339,25 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -3452,25 +3371,25 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -3481,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3502,18 +3421,42 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45">
         <v>0</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3521,25 +3464,25 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -3553,22 +3496,22 @@
         <v>0</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3581,35 +3524,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" t="s">
         <v>0</v>
       </c>
       <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3617,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -3638,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -3652,25 +3571,25 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -3699,10 +3618,10 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -3763,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -3780,25 +3699,25 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -3809,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -3830,9 +3749,105 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
         <v>0</v>
       </c>
     </row>

</xml_diff>